<commit_message>
recalculated CMIP6 GWLs with new ensemble
</commit_message>
<xml_diff>
--- a/data/gwl_lists/GWLs_CMIP5_OEKS15_fixed_periods.xlsx
+++ b/data/gwl_lists/GWLs_CMIP5_OEKS15_fixed_periods.xlsx
@@ -1,21 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbecsi/Desktop/Arbeit/Qgis/data/AAR2/GWLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6F2C47-2ECE-A246-9EE7-6751C4534265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E6208D-8FE3-E744-A691-FDB1195417B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22120" activeTab="1" xr2:uid="{1016860F-A044-804B-A1C1-209A73595C7A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" activeTab="2" xr2:uid="{1016860F-A044-804B-A1C1-209A73595C7A}"/>
   </bookViews>
   <sheets>
     <sheet name="lookup_table" sheetId="3" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
+    <sheet name="fixed_periods_RCPs" sheetId="4" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">[1]Tabelle2!$B$12:$B$19</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">[1]Tabelle2!$B$20:$B$28</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">(Tabelle1!$E$10:$E$21,Tabelle1!$E$39)</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">(Tabelle1!$E$22,Tabelle1!$E$23,Tabelle1!$E$24,Tabelle1!$E$27,Tabelle1!$E$28,Tabelle1!$E$29,Tabelle1!$E$30,Tabelle1!$E$31,Tabelle1!$E$32,Tabelle1!$E$33,Tabelle1!$E$40)</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">(Tabelle1!$E$3:$E$9,Tabelle1!$E$38)</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Tabelle1!$D$10:$D$21</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Tabelle1!$D$22:$D$33</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Tabelle1!$D$3:$D$9</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Tabelle1!$E$3:$E$9</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">[1]Tabelle2!$B$12:$B$19</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">[1]Tabelle2!$B$20:$B$28</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">[1]Tabelle2!$B$3:$B$11</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">[1]Tabelle2!$B$3:$B$11</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">[1]Tabelle2!$C$12:$C$19</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">[1]Tabelle2!$C$20:$C$28</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">[1]Tabelle2!$C$3:$C$11</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">[1]Tabelle2!$F$33:$F$42</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">(Tabelle1!$D$10:$D$21,Tabelle1!$D$39)</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">(Tabelle1!$D$22:$D$33,Tabelle1!$D$40)</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">(Tabelle1!$D$3:$D$9,Tabelle1!$D$38)</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">(Tabelle1!$E$10:$E$21,Tabelle1!$E$39)</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">(Tabelle1!$E$22,Tabelle1!$E$23,Tabelle1!$E$24,Tabelle1!$E$27,Tabelle1!$E$28,Tabelle1!$E$29,Tabelle1!$E$30,Tabelle1!$E$31,Tabelle1!$E$32,Tabelle1!$E$33,Tabelle1!$E$40)</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">(Tabelle1!$E$3:$E$9,Tabelle1!$E$38)</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">[1]Tabelle2!$C$12:$C$19</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Tabelle1!$D$10:$D$21</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Tabelle1!$D$22:$D$33</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Tabelle1!$D$3:$D$9</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Tabelle1!$E$3:$E$9</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">[1]Tabelle2!$C$20:$C$28</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">[1]Tabelle2!$C$3:$C$11</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">[1]Tabelle2!$F$33:$F$42</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">(Tabelle1!$D$10:$D$21,Tabelle1!$D$39)</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">(Tabelle1!$D$22:$D$33,Tabelle1!$D$40)</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">(Tabelle1!$D$3:$D$9,Tabelle1!$D$38)</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -235,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +291,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -291,6 +349,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -306,6 +367,1284 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.26</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.24</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.25</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3"/>
+    <cx:data id="4">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.29</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="5">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.27</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="6">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.28</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1600" b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>GWLs for three RCPs of the ÖKS15 ensemble</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1600" b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t> at mid (2041-2060) and end (2081-2100) century</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:plotSurface>
+          <cx:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </cx:spPr>
+        </cx:plotSurface>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000007-193D-854A-9500-F4E44829579D}" formatIdx="3">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Mid century RCP2.6</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000000-6095-E043-B0A1-0ED8C149B120}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Mid century RCP4.5</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000001-6095-E043-B0A1-0ED8C149B120}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Mid century RCP8.5</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000002-6095-E043-B0A1-0ED8C149B120}">
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000003-6095-E043-B0A1-0ED8C149B120}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>End century RCP2.6</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="4"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000004-6095-E043-B0A1-0ED8C149B120}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>End century RCP4.5</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="5"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000005-6095-E043-B0A1-0ED8C149B120}">
+          <cx:tx>
+            <cx:txData>
+              <cx:v>End century RCP8.5</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="6"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Global warming level</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1400"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Global warming level</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:majorTickMarks type="out"/>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="r" align="ctr" overlay="0">
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:sysClr>
+            </a:solidFill>
+            <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+          </a:endParaRPr>
+        </a:p>
+      </cx:txPr>
+    </cx:legend>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{DF10F5C8-EAEB-BA4D-A8DC-804EB02FCAAE}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9304421" cy="6015789"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Diagramm 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14546084-EB2A-5F69-D778-BA644C90A927}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks/>
+            </xdr:cNvGraphicFramePr>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+              <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Rechteck 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63F3D3DB-6F83-9E80-913C-6F6B25CFBD07}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr>
+          <a:spLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noTextEdit="1"/>
+        </cdr:cNvSpPr>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="9304421" cy="6015789"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstClr val="white"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="1">
+          <a:solidFill>
+            <a:prstClr val="green"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" horzOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Dieses Diagramm ist in Ihrer Version von Excel nicht verfügbar.
+Wenn Sie diese Form bearbeiten oder diese Arbeitsmappe in einem anderen Dateiformat speichern, wird das Diagramm dauerhaft beschädigt.</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Tabelle2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="B3">
+            <v>2008</v>
+          </cell>
+          <cell r="C3">
+            <v>2025</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>2044</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>2014</v>
+          </cell>
+          <cell r="C5">
+            <v>2034</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>2011</v>
+          </cell>
+          <cell r="C6">
+            <v>2032</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>2016</v>
+          </cell>
+          <cell r="C7">
+            <v>2047</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>2085</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>2012</v>
+          </cell>
+          <cell r="C10">
+            <v>2044</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>2023</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>2008</v>
+          </cell>
+          <cell r="C12">
+            <v>2024</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>2038</v>
+          </cell>
+          <cell r="C13">
+            <v>2059</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14">
+            <v>2018</v>
+          </cell>
+          <cell r="C14">
+            <v>2032</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15">
+            <v>2014</v>
+          </cell>
+          <cell r="C15">
+            <v>2031</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16">
+            <v>2042</v>
+          </cell>
+          <cell r="C16">
+            <v>2068</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17">
+            <v>2040</v>
+          </cell>
+          <cell r="C17">
+            <v>2074</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18">
+            <v>2012</v>
+          </cell>
+          <cell r="C18">
+            <v>2035</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19">
+            <v>2022</v>
+          </cell>
+          <cell r="C19">
+            <v>2044</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20">
+            <v>2009</v>
+          </cell>
+          <cell r="C20">
+            <v>2023</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21">
+            <v>2031</v>
+          </cell>
+          <cell r="C21">
+            <v>2046</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22">
+            <v>2014</v>
+          </cell>
+          <cell r="C22">
+            <v>2027</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23">
+            <v>2023</v>
+          </cell>
+          <cell r="C23">
+            <v>2035</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24">
+            <v>2011</v>
+          </cell>
+          <cell r="C24">
+            <v>2027</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25">
+            <v>2034</v>
+          </cell>
+          <cell r="C25">
+            <v>2048</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26">
+            <v>2033</v>
+          </cell>
+          <cell r="C26">
+            <v>2050</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27">
+            <v>2011</v>
+          </cell>
+          <cell r="C27">
+            <v>2029</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28">
+            <v>2020</v>
+          </cell>
+          <cell r="C28">
+            <v>2037</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1109,8 +2448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35341D5B-AD4F-FA40-8880-E2D5A5A65231}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1163,7 +2502,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
@@ -1189,7 +2528,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
@@ -1215,7 +2554,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
@@ -1241,7 +2580,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
@@ -1267,7 +2606,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
@@ -1293,7 +2632,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
@@ -1319,7 +2658,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
@@ -1345,7 +2684,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
@@ -1371,7 +2710,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
@@ -1397,7 +2736,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
@@ -1423,7 +2762,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B13" t="s">
@@ -1449,7 +2788,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B14" t="s">
@@ -1475,7 +2814,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B15" t="s">
@@ -1501,7 +2840,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
@@ -1527,7 +2866,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B17" t="s">
@@ -1553,7 +2892,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B18" t="s">
@@ -1579,7 +2918,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B19" t="s">
@@ -1605,7 +2944,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B20" t="s">
@@ -1631,7 +2970,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B21" t="s">
@@ -1657,7 +2996,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B22" t="s">
@@ -1683,7 +3022,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
@@ -1709,7 +3048,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B24" t="s">
@@ -1735,7 +3074,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B25" t="s">
@@ -1757,7 +3096,7 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B26" t="s">
@@ -1779,7 +3118,7 @@
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B27" t="s">
@@ -1805,7 +3144,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B28" t="s">
@@ -1831,7 +3170,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B29" t="s">
@@ -1857,7 +3196,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B30" t="s">
@@ -1883,7 +3222,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B31" t="s">
@@ -1909,7 +3248,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B32" t="s">
@@ -1935,7 +3274,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B33" t="s">

</xml_diff>